<commit_message>
ajuste de dimensao de imagem
</commit_message>
<xml_diff>
--- a/mordomo/nome-do-arquivo.xlsx
+++ b/mordomo/nome-do-arquivo.xlsx
@@ -136,7 +136,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="104775" cy="933450"/>
+    <ext cx="838200" cy="1200150"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -161,7 +161,7 @@
       <row>2</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="104775" cy="933450"/>
+    <ext cx="838200" cy="1200150"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -186,7 +186,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="104775" cy="933450"/>
+    <ext cx="838200" cy="1200150"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -211,7 +211,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="104775" cy="933450"/>
+    <ext cx="838200" cy="1200150"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -236,7 +236,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="104775" cy="933450"/>
+    <ext cx="838200" cy="1200150"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>

</xml_diff>

<commit_message>
aumentando a altura das linhas
</commit_message>
<xml_diff>
--- a/mordomo/nome-do-arquivo.xlsx
+++ b/mordomo/nome-do-arquivo.xlsx
@@ -599,7 +599,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="97.5" customHeight="1">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -627,7 +627,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="97.5" customHeight="1">
       <c r="A3" t="n">
         <v>2</v>
       </c>
@@ -655,7 +655,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="97.5" customHeight="1">
       <c r="A4" t="n">
         <v>3</v>
       </c>
@@ -683,7 +683,7 @@
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="97.5" customHeight="1">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -711,7 +711,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="97.5" customHeight="1">
       <c r="A6" t="n">
         <v>5</v>
       </c>

</xml_diff>